<commit_message>
Se acompleta informacion en diagrama de conexion
</commit_message>
<xml_diff>
--- a/Documentos/parametros suavizador magnum.xlsx
+++ b/Documentos/parametros suavizador magnum.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hh\suav-magnumcv\Documentos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="11595" windowHeight="7170"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="57">
   <si>
     <t>Suav 1</t>
   </si>
@@ -181,12 +186,18 @@
   </si>
   <si>
     <t>Tiempo Llenado</t>
+  </si>
+  <si>
+    <t>"Tiempo avance a servicio" debe ser ajustado si es que se le dejan las dos pestañas que activan el micro en el engrane (no probado completamente)</t>
+  </si>
+  <si>
+    <t>Parametros suav magnumcv con PLC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -231,7 +242,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -254,17 +265,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -282,6 +327,27 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -291,6 +357,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -339,7 +408,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -374,7 +443,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -583,594 +652,642 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="7"/>
+    <col min="4" max="4" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="1"/>
+      <c r="A1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="9" t="s">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="9" t="s">
+      <c r="D4" s="7">
+        <v>62</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="9" t="s">
+      <c r="D5" s="7">
+        <v>317</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="9" t="s">
+      <c r="D6" s="7">
+        <v>345</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="9" t="s">
+      <c r="D7" s="7">
+        <v>460</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="9" t="s">
+      <c r="D8" s="7">
+        <v>145</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D9" s="7">
         <v>10</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="9" t="s">
+      <c r="E9" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D10" s="7">
         <v>55</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="9" t="s">
+      <c r="E10" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D11" s="7">
         <v>15</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="9" t="s">
+      <c r="E11" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D12" s="7">
         <v>20</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="E12" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="9" t="s">
+    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="9" t="s">
+      <c r="D14" s="7"/>
+      <c r="E14" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="9" t="s">
+      <c r="D15" s="7"/>
+      <c r="E15" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="9" t="s">
+      <c r="D16" s="7"/>
+      <c r="E16" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="9" t="s">
+      <c r="D17" s="7"/>
+      <c r="E17" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="9" t="s">
+      <c r="D18" s="7"/>
+      <c r="E18" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D19" s="7">
         <v>10</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="9" t="s">
+      <c r="E19" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D20" s="7">
         <v>55</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="9" t="s">
+      <c r="E20" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D21" s="7">
         <v>15</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="9" t="s">
+      <c r="E21" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D22" s="7">
         <v>20</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="E22" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="9" t="s">
+    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="9" t="s">
+      <c r="D24" s="7"/>
+      <c r="E24" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="9" t="s">
+      <c r="D25" s="7"/>
+      <c r="E25" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
+      <c r="B26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="9" t="s">
+      <c r="D26" s="7"/>
+      <c r="E26" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="9" t="s">
+      <c r="D27" s="7"/>
+      <c r="E27" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="9" t="s">
+      <c r="D28" s="7"/>
+      <c r="E28" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D29" s="7">
         <v>10</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="9" t="s">
+      <c r="E29" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D30" s="7">
         <v>55</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="9" t="s">
+      <c r="E30" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+      <c r="B31" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D31" s="7">
         <v>15</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="9" t="s">
+      <c r="E31" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D32" s="7">
         <v>20</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+      <c r="E32" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B33" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="9" t="s">
+    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="9" t="s">
+      <c r="D34" s="7">
+        <v>62</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
+      <c r="B35" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="9" t="s">
+      <c r="D35" s="7">
+        <v>317</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="9" t="s">
+      <c r="D36" s="7">
+        <v>345</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="13"/>
+      <c r="B37" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="8"/>
-      <c r="E36" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="9" t="s">
+      <c r="D37" s="7">
+        <v>460</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="13"/>
+      <c r="B38" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="9" t="s">
+      <c r="D38" s="7">
+        <v>145</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="9" t="s">
+      <c r="D39" s="7">
+        <v>10</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D39" s="8"/>
-      <c r="E39" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="9" t="s">
+      <c r="D40" s="7">
+        <v>55</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="9" t="s">
+      <c r="D41" s="7">
+        <v>15</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="D42" s="7">
+        <v>20</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="A23:A31"/>
-    <mergeCell ref="A33:A41"/>
+  <mergeCells count="6">
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="A14:A22"/>
+    <mergeCell ref="A24:A32"/>
+    <mergeCell ref="A34:A42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="98" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>